<commit_message>
Enhance attendance marking and reporting features
- Implemented automatic attendance marking for recognized students, streamlining the process and reducing manual input.
- Added functionality to calculate expected classes based on weekly schedules, improving attendance reporting accuracy.
- Updated attendance summary to include expected classes, providing better insights into student attendance performance.
- Enhanced error handling and logging for attendance processing, ensuring better feedback and diagnostics for users.
</commit_message>
<xml_diff>
--- a/excel_exports/Class_Report_ENTC_B.TechB_2025-11-08_to_2025-11-22.xlsx
+++ b/excel_exports/Class_Report_ENTC_B.TechB_2025-11-08_to_2025-11-22.xlsx
@@ -490,14 +490,14 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>33.3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>91-100%</t>
+          <t>26-50%</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -548,14 +548,14 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>33.3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>91-100%</t>
+          <t>26-50%</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -633,14 +633,14 @@
         <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>91-100%</t>
+          <t>26-50%</t>
         </is>
       </c>
     </row>
@@ -664,14 +664,14 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>100</v>
+        <v>33.3</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>91-100%</t>
+          <t>26-50%</t>
         </is>
       </c>
     </row>
@@ -692,10 +692,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>100</v>
@@ -726,14 +726,14 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
-        <v>100</v>
+        <v>33.3</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>91-100%</t>
+          <t>26-50%</t>
         </is>
       </c>
     </row>

</xml_diff>